<commit_message>
modified marks for cse 104 section 1
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 208/Fall2019_CSE208_Sec1_CoPo.xlsx
+++ b/FALL 19/CSE 208/Fall2019_CSE208_Sec1_CoPo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 19\CSE 208\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30ED7EB7-854B-4B12-A1A7-7E3768EE34C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8709E377-0BDA-47EC-B8F9-4248FA287714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="744" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="744" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GradeSheet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="183">
   <si>
     <t>Numerical Grade</t>
   </si>
@@ -3045,6 +3045,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="92" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="94" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3060,17 +3084,10 @@
     <xf numFmtId="1" fontId="5" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3088,32 +3105,74 @@
     <xf numFmtId="1" fontId="4" fillId="6" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="92" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="6" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3130,74 +3189,8 @@
     <xf numFmtId="1" fontId="11" fillId="9" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="11" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3211,6 +3204,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="58" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3228,6 +3225,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -7314,35 +7314,35 @@
         <v>79</v>
       </c>
       <c r="P27" s="59">
-        <f>MAX(P10:P23)</f>
+        <f t="shared" ref="P27:W27" si="8">MAX(P10:P23)</f>
         <v>10</v>
       </c>
       <c r="Q27" s="59">
-        <f>MAX(Q10:Q23)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="R27" s="129">
-        <f>MAX(R10:R23)</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="S27" s="129">
-        <f>MAX(S10:S23)</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="T27" s="129">
-        <f>MAX(T10:T23)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U27" s="129">
-        <f>MAX(U10:U23)</f>
+        <f t="shared" si="8"/>
         <v>10.5</v>
       </c>
       <c r="V27" s="129">
-        <f>MAX(V10:V23)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="W27" s="129">
-        <f>MAX(W10:W23)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X27" s="4"/>
@@ -7381,35 +7381,35 @@
         <v>81</v>
       </c>
       <c r="P28" s="59">
-        <f>AVERAGE(P10:P23)</f>
+        <f t="shared" ref="P28:W28" si="9">AVERAGE(P10:P23)</f>
         <v>7</v>
       </c>
       <c r="Q28" s="59">
-        <f>AVERAGE(Q10:Q23)</f>
+        <f t="shared" si="9"/>
         <v>4.0714285714285712</v>
       </c>
       <c r="R28" s="59">
-        <f>AVERAGE(R10:R23)</f>
+        <f t="shared" si="9"/>
         <v>6.3571428571428568</v>
       </c>
       <c r="S28" s="59">
-        <f>AVERAGE(S10:S23)</f>
+        <f t="shared" si="9"/>
         <v>2.2857142857142856</v>
       </c>
       <c r="T28" s="59">
-        <f>AVERAGE(T10:T23)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U28" s="59">
-        <f>AVERAGE(U10:U23)</f>
+        <f t="shared" si="9"/>
         <v>4.7142857142857144</v>
       </c>
       <c r="V28" s="59">
-        <f>AVERAGE(V10:V23)</f>
+        <f t="shared" si="9"/>
         <v>3.4642857142857144</v>
       </c>
       <c r="W28" s="59">
-        <f>AVERAGE(W10:W23)</f>
+        <f t="shared" si="9"/>
         <v>1.2857142857142858</v>
       </c>
       <c r="X28" s="4"/>
@@ -7448,35 +7448,35 @@
         <v>84</v>
       </c>
       <c r="P29" s="59">
-        <f>MIN(P10:P23)</f>
+        <f t="shared" ref="P29:W29" si="10">MIN(P10:P23)</f>
         <v>0</v>
       </c>
       <c r="Q29" s="59">
-        <f>MIN(Q10:Q23)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="R29" s="129">
-        <f>MIN(R10:R23)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S29" s="129">
-        <f>MIN(S10:S23)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T29" s="129">
-        <f>MIN(T10:T23)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="U29" s="129">
-        <f>MIN(U10:U23)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V29" s="129">
-        <f>MIN(V10:V23)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="W29" s="129">
-        <f>MIN(W10:W23)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="X29" s="4"/>
@@ -21054,8 +21054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BR1015"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="AN7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="BD36" sqref="BD36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15" customHeight="1"/>
@@ -21084,7 +21084,7 @@
     <row r="1" spans="1:70" ht="13.8">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="258"/>
+      <c r="C1" s="270"/>
       <c r="D1" s="254"/>
       <c r="E1" s="254"/>
       <c r="F1" s="254"/>
@@ -21510,21 +21510,21 @@
       <c r="AP7" s="3"/>
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
-      <c r="AS7" s="255" t="s">
+      <c r="AS7" s="267" t="s">
         <v>4</v>
       </c>
-      <c r="AT7" s="256"/>
-      <c r="AU7" s="256"/>
-      <c r="AV7" s="256"/>
-      <c r="AW7" s="256"/>
-      <c r="AX7" s="256"/>
-      <c r="AY7" s="256"/>
-      <c r="AZ7" s="256"/>
-      <c r="BA7" s="256"/>
-      <c r="BB7" s="256"/>
-      <c r="BC7" s="256"/>
-      <c r="BD7" s="256"/>
-      <c r="BE7" s="257"/>
+      <c r="AT7" s="268"/>
+      <c r="AU7" s="268"/>
+      <c r="AV7" s="268"/>
+      <c r="AW7" s="268"/>
+      <c r="AX7" s="268"/>
+      <c r="AY7" s="268"/>
+      <c r="AZ7" s="268"/>
+      <c r="BA7" s="268"/>
+      <c r="BB7" s="268"/>
+      <c r="BC7" s="268"/>
+      <c r="BD7" s="268"/>
+      <c r="BE7" s="269"/>
       <c r="BF7" s="205"/>
       <c r="BG7" s="205"/>
       <c r="BH7" s="3"/>
@@ -22420,12 +22420,12 @@
       <c r="BR16" s="3"/>
     </row>
     <row r="17" spans="1:70" ht="14.4" thickBot="1">
-      <c r="A17" s="271" t="str">
+      <c r="A17" s="278" t="str">
         <f>CONCATENATE("Course Outcome (CO) Attainment Analysis of ",GradeSheet!$H$2, " [",GradeSheet!$H$3, "] ", "(Section ",GradeSheet!$L$2, ") ", "[Semester - ",GradeSheet!$L$3,"]" )</f>
         <v>Course Outcome (CO) Attainment Analysis of CSE 208 [Data Structure Lab] (Section 1) [Semester - Fall 2019]</v>
       </c>
-      <c r="B17" s="264"/>
-      <c r="C17" s="265"/>
+      <c r="B17" s="259"/>
+      <c r="C17" s="260"/>
       <c r="D17" s="134"/>
       <c r="E17" s="134"/>
       <c r="F17" s="134"/>
@@ -22450,149 +22450,150 @@
       <c r="Y17" s="134"/>
       <c r="Z17" s="134"/>
       <c r="AA17" s="141"/>
-      <c r="AB17" s="267" t="s">
+      <c r="AB17" s="274" t="s">
         <v>48</v>
       </c>
-      <c r="AC17" s="262"/>
-      <c r="AD17" s="262"/>
-      <c r="AE17" s="262"/>
-      <c r="AF17" s="262"/>
-      <c r="AG17" s="262"/>
-      <c r="AH17" s="262"/>
-      <c r="AI17" s="262"/>
-      <c r="AJ17" s="262"/>
-      <c r="AK17" s="262"/>
-      <c r="AL17" s="262"/>
-      <c r="AM17" s="262"/>
-      <c r="AN17" s="262"/>
-      <c r="AO17" s="262"/>
-      <c r="AP17" s="262"/>
-      <c r="AQ17" s="262"/>
-      <c r="AR17" s="262"/>
-      <c r="AS17" s="260"/>
+      <c r="AC17" s="265"/>
+      <c r="AD17" s="265"/>
+      <c r="AE17" s="265"/>
+      <c r="AF17" s="265"/>
+      <c r="AG17" s="265"/>
+      <c r="AH17" s="265"/>
+      <c r="AI17" s="265"/>
+      <c r="AJ17" s="265"/>
+      <c r="AK17" s="265"/>
+      <c r="AL17" s="265"/>
+      <c r="AM17" s="265"/>
+      <c r="AN17" s="265"/>
+      <c r="AO17" s="265"/>
+      <c r="AP17" s="265"/>
+      <c r="AQ17" s="265"/>
+      <c r="AR17" s="265"/>
+      <c r="AS17" s="266"/>
       <c r="AT17" s="33"/>
-      <c r="AU17" s="261" t="s">
+      <c r="AU17" s="272" t="s">
         <v>50</v>
       </c>
-      <c r="AV17" s="262"/>
-      <c r="AW17" s="262"/>
-      <c r="AX17" s="262"/>
-      <c r="AY17" s="262"/>
-      <c r="AZ17" s="262"/>
-      <c r="BA17" s="262"/>
-      <c r="BB17" s="262"/>
-      <c r="BC17" s="262"/>
-      <c r="BD17" s="262"/>
-      <c r="BE17" s="262"/>
-      <c r="BF17" s="262"/>
-      <c r="BG17" s="262"/>
-      <c r="BH17" s="262"/>
-      <c r="BI17" s="262"/>
-      <c r="BJ17" s="262"/>
-      <c r="BK17" s="262"/>
-      <c r="BL17" s="262"/>
-      <c r="BM17" s="262"/>
-      <c r="BN17" s="262"/>
-      <c r="BO17" s="262"/>
-      <c r="BP17" s="262"/>
-      <c r="BQ17" s="262"/>
-      <c r="BR17" s="260"/>
+      <c r="AV17" s="265"/>
+      <c r="AW17" s="265"/>
+      <c r="AX17" s="265"/>
+      <c r="AY17" s="265"/>
+      <c r="AZ17" s="265"/>
+      <c r="BA17" s="265"/>
+      <c r="BB17" s="265"/>
+      <c r="BC17" s="265"/>
+      <c r="BD17" s="265"/>
+      <c r="BE17" s="265"/>
+      <c r="BF17" s="265"/>
+      <c r="BG17" s="265"/>
+      <c r="BH17" s="265"/>
+      <c r="BI17" s="265"/>
+      <c r="BJ17" s="265"/>
+      <c r="BK17" s="265"/>
+      <c r="BL17" s="265"/>
+      <c r="BM17" s="265"/>
+      <c r="BN17" s="265"/>
+      <c r="BO17" s="265"/>
+      <c r="BP17" s="265"/>
+      <c r="BQ17" s="265"/>
+      <c r="BR17" s="266"/>
     </row>
     <row r="18" spans="1:70" ht="14.4" thickBot="1">
-      <c r="A18" s="272"/>
+      <c r="A18" s="279"/>
       <c r="B18" s="254"/>
       <c r="C18" s="252"/>
-      <c r="D18" s="268" t="str">
+      <c r="D18" s="275" t="str">
         <f>C9</f>
         <v>Midterm Exam</v>
       </c>
-      <c r="E18" s="269"/>
-      <c r="F18" s="269"/>
-      <c r="G18" s="269"/>
-      <c r="H18" s="269"/>
-      <c r="I18" s="270"/>
-      <c r="J18" s="268" t="str">
+      <c r="E18" s="276"/>
+      <c r="F18" s="276"/>
+      <c r="G18" s="276"/>
+      <c r="H18" s="276"/>
+      <c r="I18" s="277"/>
+      <c r="J18" s="275" t="str">
         <f>C10</f>
         <v>Final Exam</v>
       </c>
-      <c r="K18" s="269"/>
-      <c r="L18" s="269"/>
-      <c r="M18" s="269"/>
-      <c r="N18" s="269"/>
-      <c r="O18" s="270"/>
-      <c r="P18" s="268" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q18" s="269"/>
-      <c r="R18" s="269"/>
-      <c r="S18" s="269"/>
-      <c r="T18" s="269"/>
-      <c r="U18" s="270"/>
-      <c r="V18" s="268" t="str">
+      <c r="K18" s="276"/>
+      <c r="L18" s="276"/>
+      <c r="M18" s="276"/>
+      <c r="N18" s="276"/>
+      <c r="O18" s="277"/>
+      <c r="P18" s="275" t="str">
+        <f>C11</f>
+        <v>Project</v>
+      </c>
+      <c r="Q18" s="276"/>
+      <c r="R18" s="276"/>
+      <c r="S18" s="276"/>
+      <c r="T18" s="276"/>
+      <c r="U18" s="277"/>
+      <c r="V18" s="275" t="str">
         <f>C12</f>
         <v>Quiz</v>
       </c>
-      <c r="W18" s="269"/>
-      <c r="X18" s="269"/>
-      <c r="Y18" s="269"/>
-      <c r="Z18" s="269"/>
-      <c r="AA18" s="270"/>
-      <c r="AB18" s="263" t="s">
+      <c r="W18" s="276"/>
+      <c r="X18" s="276"/>
+      <c r="Y18" s="276"/>
+      <c r="Z18" s="276"/>
+      <c r="AA18" s="277"/>
+      <c r="AB18" s="273" t="s">
         <v>60</v>
       </c>
-      <c r="AC18" s="264"/>
-      <c r="AD18" s="264"/>
-      <c r="AE18" s="264"/>
-      <c r="AF18" s="264"/>
-      <c r="AG18" s="265"/>
-      <c r="AH18" s="266" t="s">
+      <c r="AC18" s="259"/>
+      <c r="AD18" s="259"/>
+      <c r="AE18" s="259"/>
+      <c r="AF18" s="259"/>
+      <c r="AG18" s="260"/>
+      <c r="AH18" s="264" t="s">
         <v>63</v>
       </c>
-      <c r="AI18" s="262"/>
-      <c r="AJ18" s="262"/>
-      <c r="AK18" s="262"/>
-      <c r="AL18" s="262"/>
-      <c r="AM18" s="260"/>
-      <c r="AN18" s="266" t="s">
+      <c r="AI18" s="265"/>
+      <c r="AJ18" s="265"/>
+      <c r="AK18" s="265"/>
+      <c r="AL18" s="265"/>
+      <c r="AM18" s="266"/>
+      <c r="AN18" s="264" t="s">
         <v>66</v>
       </c>
-      <c r="AO18" s="262"/>
-      <c r="AP18" s="262"/>
-      <c r="AQ18" s="262"/>
-      <c r="AR18" s="262"/>
-      <c r="AS18" s="260"/>
+      <c r="AO18" s="265"/>
+      <c r="AP18" s="265"/>
+      <c r="AQ18" s="265"/>
+      <c r="AR18" s="265"/>
+      <c r="AS18" s="266"/>
       <c r="AT18" s="33"/>
-      <c r="AU18" s="280" t="s">
+      <c r="AU18" s="258" t="s">
         <v>63</v>
       </c>
-      <c r="AV18" s="264"/>
-      <c r="AW18" s="264"/>
-      <c r="AX18" s="264"/>
-      <c r="AY18" s="264"/>
-      <c r="AZ18" s="264"/>
-      <c r="BA18" s="264"/>
-      <c r="BB18" s="264"/>
-      <c r="BC18" s="264"/>
-      <c r="BD18" s="264"/>
-      <c r="BE18" s="264"/>
-      <c r="BF18" s="265"/>
-      <c r="BG18" s="280" t="s">
+      <c r="AV18" s="259"/>
+      <c r="AW18" s="259"/>
+      <c r="AX18" s="259"/>
+      <c r="AY18" s="259"/>
+      <c r="AZ18" s="259"/>
+      <c r="BA18" s="259"/>
+      <c r="BB18" s="259"/>
+      <c r="BC18" s="259"/>
+      <c r="BD18" s="259"/>
+      <c r="BE18" s="259"/>
+      <c r="BF18" s="260"/>
+      <c r="BG18" s="258" t="s">
         <v>67</v>
       </c>
-      <c r="BH18" s="264"/>
-      <c r="BI18" s="264"/>
-      <c r="BJ18" s="264"/>
-      <c r="BK18" s="264"/>
-      <c r="BL18" s="264"/>
-      <c r="BM18" s="264"/>
-      <c r="BN18" s="264"/>
-      <c r="BO18" s="264"/>
-      <c r="BP18" s="264"/>
-      <c r="BQ18" s="264"/>
-      <c r="BR18" s="265"/>
+      <c r="BH18" s="259"/>
+      <c r="BI18" s="259"/>
+      <c r="BJ18" s="259"/>
+      <c r="BK18" s="259"/>
+      <c r="BL18" s="259"/>
+      <c r="BM18" s="259"/>
+      <c r="BN18" s="259"/>
+      <c r="BO18" s="259"/>
+      <c r="BP18" s="259"/>
+      <c r="BQ18" s="259"/>
+      <c r="BR18" s="260"/>
     </row>
     <row r="19" spans="1:70" ht="14.4" thickBot="1">
-      <c r="A19" s="272"/>
+      <c r="A19" s="279"/>
       <c r="B19" s="252"/>
       <c r="C19" s="252"/>
       <c r="D19" s="135" t="s">
@@ -22943,14 +22944,14 @@
       <c r="AM20" s="65">
         <v>1</v>
       </c>
-      <c r="AN20" s="279" t="s">
+      <c r="AN20" s="255" t="s">
         <v>72</v>
       </c>
-      <c r="AO20" s="274"/>
-      <c r="AP20" s="274"/>
-      <c r="AQ20" s="274"/>
-      <c r="AR20" s="274"/>
-      <c r="AS20" s="275"/>
+      <c r="AO20" s="256"/>
+      <c r="AP20" s="256"/>
+      <c r="AQ20" s="256"/>
+      <c r="AR20" s="256"/>
+      <c r="AS20" s="257"/>
       <c r="AT20" s="56"/>
       <c r="AU20" s="63">
         <v>1</v>
@@ -22988,20 +22989,20 @@
       <c r="BF20" s="65">
         <v>1</v>
       </c>
-      <c r="BG20" s="273" t="s">
+      <c r="BG20" s="280" t="s">
         <v>73</v>
       </c>
-      <c r="BH20" s="274"/>
-      <c r="BI20" s="274"/>
-      <c r="BJ20" s="274"/>
-      <c r="BK20" s="274"/>
-      <c r="BL20" s="274"/>
-      <c r="BM20" s="274"/>
-      <c r="BN20" s="274"/>
-      <c r="BO20" s="274"/>
-      <c r="BP20" s="274"/>
-      <c r="BQ20" s="274"/>
-      <c r="BR20" s="275"/>
+      <c r="BH20" s="256"/>
+      <c r="BI20" s="256"/>
+      <c r="BJ20" s="256"/>
+      <c r="BK20" s="256"/>
+      <c r="BL20" s="256"/>
+      <c r="BM20" s="256"/>
+      <c r="BN20" s="256"/>
+      <c r="BO20" s="256"/>
+      <c r="BP20" s="256"/>
+      <c r="BQ20" s="256"/>
+      <c r="BR20" s="257"/>
     </row>
     <row r="21" spans="1:70" ht="16.2" thickBot="1">
       <c r="A21" s="158">
@@ -26599,14 +26600,14 @@
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
       <c r="AM35" s="3"/>
-      <c r="AN35" s="276" t="s">
+      <c r="AN35" s="261" t="s">
         <v>153</v>
       </c>
-      <c r="AO35" s="281"/>
-      <c r="AP35" s="281"/>
-      <c r="AQ35" s="281"/>
-      <c r="AR35" s="281"/>
-      <c r="AS35" s="282"/>
+      <c r="AO35" s="262"/>
+      <c r="AP35" s="262"/>
+      <c r="AQ35" s="262"/>
+      <c r="AR35" s="262"/>
+      <c r="AS35" s="263"/>
       <c r="AT35" s="33"/>
       <c r="AU35" s="122"/>
       <c r="AV35" s="3"/>
@@ -26620,148 +26621,148 @@
       <c r="BD35" s="3"/>
       <c r="BE35" s="3"/>
       <c r="BF35" s="3"/>
-      <c r="BG35" s="276" t="s">
+      <c r="BG35" s="261" t="s">
         <v>154</v>
       </c>
-      <c r="BH35" s="277"/>
-      <c r="BI35" s="277"/>
-      <c r="BJ35" s="277"/>
-      <c r="BK35" s="277"/>
-      <c r="BL35" s="277"/>
-      <c r="BM35" s="277"/>
-      <c r="BN35" s="277"/>
-      <c r="BO35" s="277"/>
-      <c r="BP35" s="277"/>
-      <c r="BQ35" s="277"/>
-      <c r="BR35" s="278"/>
+      <c r="BH35" s="281"/>
+      <c r="BI35" s="281"/>
+      <c r="BJ35" s="281"/>
+      <c r="BK35" s="281"/>
+      <c r="BL35" s="281"/>
+      <c r="BM35" s="281"/>
+      <c r="BN35" s="281"/>
+      <c r="BO35" s="281"/>
+      <c r="BP35" s="281"/>
+      <c r="BQ35" s="281"/>
+      <c r="BR35" s="282"/>
     </row>
     <row r="36" spans="1:70" ht="15.75" customHeight="1" thickBot="1">
       <c r="A36" s="123">
         <f>COUNTA(A21:A34)</f>
         <v>14</v>
       </c>
-      <c r="B36" s="259" t="s">
+      <c r="B36" s="271" t="s">
         <v>155</v>
       </c>
-      <c r="C36" s="260"/>
+      <c r="C36" s="266"/>
       <c r="D36" s="124">
-        <f>AVERAGE(D21:D34)</f>
+        <f t="shared" ref="D36:AG36" si="19">AVERAGE(D21:D34)</f>
         <v>4.7142857142857144</v>
       </c>
       <c r="E36" s="124">
-        <f>AVERAGE(E21:E34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F36" s="124">
-        <f>AVERAGE(F21:F34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="G36" s="124">
-        <f>AVERAGE(G21:G34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H36" s="124">
-        <f>AVERAGE(H21:H34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="I36" s="125">
-        <f>AVERAGE(I21:I34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J36" s="124">
-        <f>AVERAGE(J21:J34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K36" s="124">
-        <f>AVERAGE(K21:K34)</f>
+        <f t="shared" si="19"/>
         <v>1.2857142857142858</v>
       </c>
       <c r="L36" s="124">
-        <f>AVERAGE(L21:L34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M36" s="124">
-        <f>AVERAGE(M21:M34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N36" s="124">
-        <f>AVERAGE(N21:N34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O36" s="124">
-        <f>AVERAGE(O21:O34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="P36" s="124">
-        <f>AVERAGE(P21:P34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q36" s="124">
-        <f>AVERAGE(Q21:Q34)</f>
+        <f t="shared" si="19"/>
         <v>3.5</v>
       </c>
       <c r="R36" s="124">
-        <f>AVERAGE(R21:R34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="S36" s="124">
-        <f>AVERAGE(S21:S34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="T36" s="124">
-        <f>AVERAGE(T21:T34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="U36" s="124">
-        <f>AVERAGE(U21:U34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V36" s="124">
-        <f>AVERAGE(V21:V34)</f>
+        <f t="shared" si="19"/>
         <v>4.5</v>
       </c>
       <c r="W36" s="124">
-        <f>AVERAGE(W21:W34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X36" s="124">
-        <f>AVERAGE(X21:X34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y36" s="124">
-        <f>AVERAGE(Y21:Y34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z36" s="124">
-        <f>AVERAGE(Z21:Z34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA36" s="124">
-        <f>AVERAGE(AA21:AA34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB36" s="124">
-        <f>AVERAGE(AB21:AB34)</f>
+        <f t="shared" si="19"/>
         <v>9.2142857142857135</v>
       </c>
       <c r="AC36" s="124">
-        <f>AVERAGE(AC21:AC34)</f>
+        <f t="shared" si="19"/>
         <v>4.7857142857142856</v>
       </c>
       <c r="AD36" s="124">
-        <f>AVERAGE(AD21:AD34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE36" s="124">
-        <f>AVERAGE(AE21:AE34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AF36" s="124">
-        <f>AVERAGE(AF21:AF34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AG36" s="124">
-        <f>AVERAGE(AG21:AG34)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AH36" s="61">
@@ -26789,27 +26790,27 @@
         <v>0</v>
       </c>
       <c r="AN36" s="57">
-        <f>SUM(AN21:AN34)</f>
+        <f t="shared" ref="AN36:AS36" si="20">SUM(AN21:AN34)</f>
         <v>0</v>
       </c>
       <c r="AO36" s="57">
-        <f>SUM(AO21:AO34)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP36" s="57">
-        <f>SUM(AP21:AP34)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AQ36" s="57">
-        <f>SUM(AQ21:AQ34)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AR36" s="58">
-        <f>SUM(AR21:AR34)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AS36" s="58">
-        <f>SUM(AS21:AS34)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AT36" s="56"/>
@@ -26862,51 +26863,51 @@
         <v>0</v>
       </c>
       <c r="BG36" s="57">
-        <f>SUM(BG21:BG34)</f>
+        <f t="shared" ref="BG36:BR36" si="21">SUM(BG21:BG34)</f>
         <v>0</v>
       </c>
       <c r="BH36" s="57">
-        <f>SUM(BH21:BH34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BI36" s="57">
-        <f>SUM(BI21:BI34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BJ36" s="57">
-        <f>SUM(BJ21:BJ34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BK36" s="58">
-        <f>SUM(BK21:BK34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BL36" s="58">
-        <f>SUM(BL21:BL34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BM36" s="58">
-        <f>SUM(BM21:BM34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BN36" s="58">
-        <f>SUM(BN21:BN34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BO36" s="58">
-        <f>SUM(BO21:BO34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BP36" s="58">
-        <f>SUM(BP21:BP34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BQ36" s="58">
-        <f>SUM(BQ21:BQ34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BR36" s="126">
-        <f>SUM(BR21:BR34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -43569,11 +43570,6 @@
     <row r="1015" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="AN20:AS20"/>
-    <mergeCell ref="AU18:BF18"/>
-    <mergeCell ref="BG18:BR18"/>
-    <mergeCell ref="AN35:AS35"/>
-    <mergeCell ref="AN18:AS18"/>
     <mergeCell ref="AS7:BE7"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="B41:C41"/>
@@ -43590,6 +43586,11 @@
     <mergeCell ref="D18:I18"/>
     <mergeCell ref="BG20:BR20"/>
     <mergeCell ref="BG35:BR35"/>
+    <mergeCell ref="AN20:AS20"/>
+    <mergeCell ref="AU18:BF18"/>
+    <mergeCell ref="BG18:BR18"/>
+    <mergeCell ref="AN35:AS35"/>
+    <mergeCell ref="AN18:AS18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="39" orientation="landscape" r:id="rId1"/>
@@ -43606,7 +43607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AT1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="V32" sqref="V32:AH32"/>
     </sheetView>
   </sheetViews>
@@ -43688,12 +43689,12 @@
     </row>
     <row r="2" spans="1:46" ht="16.5" customHeight="1">
       <c r="A2" s="78"/>
-      <c r="B2" s="303" t="s">
+      <c r="B2" s="300" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="248"/>
       <c r="D2" s="249"/>
-      <c r="E2" s="305" t="str">
+      <c r="E2" s="302" t="str">
         <f>GradeSheet!$H$2</f>
         <v>CSE 208</v>
       </c>
@@ -43708,7 +43709,7 @@
       <c r="N2" s="248"/>
       <c r="O2" s="248"/>
       <c r="P2" s="249"/>
-      <c r="Q2" s="303" t="str">
+      <c r="Q2" s="300" t="str">
         <f>CONCATENATE("Section ", GradeSheet!$L$2,)</f>
         <v>Section 1</v>
       </c>
@@ -43716,7 +43717,7 @@
       <c r="S2" s="249"/>
       <c r="T2" s="79"/>
       <c r="U2" s="78"/>
-      <c r="V2" s="294" t="s">
+      <c r="V2" s="286" t="s">
         <v>97</v>
       </c>
       <c r="W2" s="248"/>
@@ -43746,12 +43747,12 @@
     </row>
     <row r="3" spans="1:46" ht="16.5" customHeight="1">
       <c r="A3" s="78"/>
-      <c r="B3" s="302" t="s">
+      <c r="B3" s="301" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="248"/>
       <c r="D3" s="249"/>
-      <c r="E3" s="304" t="str">
+      <c r="E3" s="299" t="str">
         <f>GradeSheet!$H$3</f>
         <v>Data Structure Lab</v>
       </c>
@@ -43766,7 +43767,7 @@
       <c r="N3" s="248"/>
       <c r="O3" s="248"/>
       <c r="P3" s="249"/>
-      <c r="Q3" s="302" t="str">
+      <c r="Q3" s="301" t="str">
         <f>CONCATENATE(GradeSheet!$H$39," students")</f>
         <v>14 students</v>
       </c>
@@ -43774,7 +43775,7 @@
       <c r="S3" s="249"/>
       <c r="T3" s="79"/>
       <c r="U3" s="78"/>
-      <c r="V3" s="285" t="s">
+      <c r="V3" s="283" t="s">
         <v>98</v>
       </c>
       <c r="W3" s="248"/>
@@ -43789,7 +43790,7 @@
       <c r="AF3" s="248"/>
       <c r="AG3" s="248"/>
       <c r="AH3" s="249"/>
-      <c r="AI3" s="285" t="s">
+      <c r="AI3" s="283" t="s">
         <v>99</v>
       </c>
       <c r="AJ3" s="248"/>
@@ -43806,12 +43807,12 @@
     </row>
     <row r="4" spans="1:46" ht="16.5" customHeight="1">
       <c r="A4" s="78"/>
-      <c r="B4" s="301" t="s">
+      <c r="B4" s="305" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="248"/>
       <c r="D4" s="249"/>
-      <c r="E4" s="300">
+      <c r="E4" s="304">
         <f>GradeSheet!$H$4</f>
         <v>3</v>
       </c>
@@ -43826,7 +43827,7 @@
       <c r="N4" s="248"/>
       <c r="O4" s="248"/>
       <c r="P4" s="249"/>
-      <c r="Q4" s="300" t="str">
+      <c r="Q4" s="304" t="str">
         <f>GradeSheet!$L$3</f>
         <v>Fall 2019</v>
       </c>
@@ -43834,7 +43835,7 @@
       <c r="S4" s="249"/>
       <c r="T4" s="79"/>
       <c r="U4" s="78"/>
-      <c r="V4" s="306">
+      <c r="V4" s="303">
         <v>1</v>
       </c>
       <c r="W4" s="248"/>
@@ -43849,7 +43850,7 @@
       <c r="AF4" s="248"/>
       <c r="AG4" s="248"/>
       <c r="AH4" s="249"/>
-      <c r="AI4" s="284">
+      <c r="AI4" s="295">
         <v>4</v>
       </c>
       <c r="AJ4" s="248"/>
@@ -43886,7 +43887,7 @@
       <c r="S5" s="81"/>
       <c r="T5" s="79"/>
       <c r="U5" s="78"/>
-      <c r="V5" s="306">
+      <c r="V5" s="303">
         <v>2</v>
       </c>
       <c r="W5" s="248"/>
@@ -43901,7 +43902,7 @@
       <c r="AF5" s="248"/>
       <c r="AG5" s="248"/>
       <c r="AH5" s="249"/>
-      <c r="AI5" s="284">
+      <c r="AI5" s="295">
         <v>4</v>
       </c>
       <c r="AJ5" s="248"/>
@@ -43938,7 +43939,7 @@
       <c r="S6" s="82"/>
       <c r="T6" s="82"/>
       <c r="U6" s="82"/>
-      <c r="V6" s="284">
+      <c r="V6" s="295">
         <v>3</v>
       </c>
       <c r="W6" s="248"/>
@@ -43953,7 +43954,7 @@
       <c r="AF6" s="248"/>
       <c r="AG6" s="248"/>
       <c r="AH6" s="249"/>
-      <c r="AI6" s="284">
+      <c r="AI6" s="295">
         <v>4</v>
       </c>
       <c r="AJ6" s="248"/>
@@ -43990,7 +43991,7 @@
       <c r="S7" s="82"/>
       <c r="T7" s="82"/>
       <c r="U7" s="82"/>
-      <c r="V7" s="284">
+      <c r="V7" s="295">
         <v>4</v>
       </c>
       <c r="W7" s="248"/>
@@ -44005,7 +44006,7 @@
       <c r="AF7" s="248"/>
       <c r="AG7" s="248"/>
       <c r="AH7" s="249"/>
-      <c r="AI7" s="284">
+      <c r="AI7" s="295">
         <v>3</v>
       </c>
       <c r="AJ7" s="248"/>
@@ -44042,7 +44043,7 @@
       <c r="S8" s="82"/>
       <c r="T8" s="82"/>
       <c r="U8" s="82"/>
-      <c r="V8" s="284">
+      <c r="V8" s="295">
         <v>5</v>
       </c>
       <c r="W8" s="248"/>
@@ -44057,7 +44058,7 @@
       <c r="AF8" s="248"/>
       <c r="AG8" s="248"/>
       <c r="AH8" s="249"/>
-      <c r="AI8" s="284">
+      <c r="AI8" s="295">
         <v>3</v>
       </c>
       <c r="AJ8" s="248"/>
@@ -44094,7 +44095,7 @@
       <c r="S9" s="82"/>
       <c r="T9" s="82"/>
       <c r="U9" s="82"/>
-      <c r="V9" s="284">
+      <c r="V9" s="295">
         <v>6</v>
       </c>
       <c r="W9" s="248"/>
@@ -44109,7 +44110,7 @@
       <c r="AF9" s="248"/>
       <c r="AG9" s="248"/>
       <c r="AH9" s="249"/>
-      <c r="AI9" s="284">
+      <c r="AI9" s="295">
         <v>3</v>
       </c>
       <c r="AJ9" s="248"/>
@@ -44146,7 +44147,7 @@
       <c r="S10" s="82"/>
       <c r="T10" s="82"/>
       <c r="U10" s="82"/>
-      <c r="V10" s="284">
+      <c r="V10" s="295">
         <v>7</v>
       </c>
       <c r="W10" s="248"/>
@@ -44161,7 +44162,7 @@
       <c r="AF10" s="248"/>
       <c r="AG10" s="248"/>
       <c r="AH10" s="249"/>
-      <c r="AI10" s="284">
+      <c r="AI10" s="295">
         <v>3</v>
       </c>
       <c r="AJ10" s="248"/>
@@ -44198,7 +44199,7 @@
       <c r="S11" s="82"/>
       <c r="T11" s="82"/>
       <c r="U11" s="82"/>
-      <c r="V11" s="284"/>
+      <c r="V11" s="295"/>
       <c r="W11" s="248"/>
       <c r="X11" s="248"/>
       <c r="Y11" s="248"/>
@@ -44211,7 +44212,7 @@
       <c r="AF11" s="248"/>
       <c r="AG11" s="248"/>
       <c r="AH11" s="249"/>
-      <c r="AI11" s="284"/>
+      <c r="AI11" s="295"/>
       <c r="AJ11" s="248"/>
       <c r="AK11" s="248"/>
       <c r="AL11" s="248"/>
@@ -44246,7 +44247,7 @@
       <c r="S12" s="82"/>
       <c r="T12" s="82"/>
       <c r="U12" s="82"/>
-      <c r="V12" s="284"/>
+      <c r="V12" s="295"/>
       <c r="W12" s="248"/>
       <c r="X12" s="248"/>
       <c r="Y12" s="248"/>
@@ -44259,7 +44260,7 @@
       <c r="AF12" s="248"/>
       <c r="AG12" s="248"/>
       <c r="AH12" s="249"/>
-      <c r="AI12" s="284"/>
+      <c r="AI12" s="295"/>
       <c r="AJ12" s="248"/>
       <c r="AK12" s="248"/>
       <c r="AL12" s="248"/>
@@ -44401,7 +44402,7 @@
       </c>
       <c r="Y15" s="254"/>
       <c r="Z15" s="254"/>
-      <c r="AA15" s="317" t="s">
+      <c r="AA15" s="297" t="s">
         <v>103</v>
       </c>
       <c r="AB15" s="249"/>
@@ -44414,7 +44415,7 @@
       </c>
       <c r="AF15" s="254"/>
       <c r="AG15" s="254"/>
-      <c r="AH15" s="285"/>
+      <c r="AH15" s="283"/>
       <c r="AI15" s="248"/>
       <c r="AJ15" s="249"/>
       <c r="AK15" s="82"/>
@@ -44424,7 +44425,7 @@
       <c r="AM15" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="AN15" s="285"/>
+      <c r="AN15" s="283"/>
       <c r="AO15" s="249"/>
       <c r="AP15" s="83"/>
       <c r="AQ15" s="84"/>
@@ -44504,30 +44505,30 @@
       <c r="S17" s="82"/>
       <c r="T17" s="82"/>
       <c r="U17" s="82"/>
-      <c r="V17" s="310"/>
-      <c r="W17" s="311"/>
-      <c r="X17" s="311"/>
-      <c r="Y17" s="311"/>
-      <c r="Z17" s="311"/>
-      <c r="AA17" s="311"/>
-      <c r="AB17" s="311"/>
-      <c r="AC17" s="311"/>
-      <c r="AD17" s="311"/>
-      <c r="AE17" s="311"/>
-      <c r="AF17" s="311"/>
-      <c r="AG17" s="311"/>
-      <c r="AH17" s="311"/>
-      <c r="AI17" s="311"/>
-      <c r="AJ17" s="311"/>
-      <c r="AK17" s="311"/>
-      <c r="AL17" s="311"/>
-      <c r="AM17" s="311"/>
-      <c r="AN17" s="311"/>
-      <c r="AO17" s="311"/>
-      <c r="AP17" s="311"/>
-      <c r="AQ17" s="311"/>
-      <c r="AR17" s="311"/>
-      <c r="AS17" s="312"/>
+      <c r="V17" s="287"/>
+      <c r="W17" s="288"/>
+      <c r="X17" s="288"/>
+      <c r="Y17" s="288"/>
+      <c r="Z17" s="288"/>
+      <c r="AA17" s="288"/>
+      <c r="AB17" s="288"/>
+      <c r="AC17" s="288"/>
+      <c r="AD17" s="288"/>
+      <c r="AE17" s="288"/>
+      <c r="AF17" s="288"/>
+      <c r="AG17" s="288"/>
+      <c r="AH17" s="288"/>
+      <c r="AI17" s="288"/>
+      <c r="AJ17" s="288"/>
+      <c r="AK17" s="288"/>
+      <c r="AL17" s="288"/>
+      <c r="AM17" s="288"/>
+      <c r="AN17" s="288"/>
+      <c r="AO17" s="288"/>
+      <c r="AP17" s="288"/>
+      <c r="AQ17" s="288"/>
+      <c r="AR17" s="288"/>
+      <c r="AS17" s="289"/>
       <c r="AT17" s="82"/>
     </row>
     <row r="18" spans="1:46" ht="16.5" customHeight="1">
@@ -44552,7 +44553,7 @@
       <c r="S18" s="82"/>
       <c r="T18" s="82"/>
       <c r="U18" s="82"/>
-      <c r="V18" s="313"/>
+      <c r="V18" s="290"/>
       <c r="W18" s="254"/>
       <c r="X18" s="254"/>
       <c r="Y18" s="254"/>
@@ -44575,7 +44576,7 @@
       <c r="AP18" s="254"/>
       <c r="AQ18" s="254"/>
       <c r="AR18" s="254"/>
-      <c r="AS18" s="314"/>
+      <c r="AS18" s="291"/>
       <c r="AT18" s="82"/>
     </row>
     <row r="19" spans="1:46" ht="16.5" customHeight="1">
@@ -44600,30 +44601,30 @@
       <c r="S19" s="82"/>
       <c r="T19" s="82"/>
       <c r="U19" s="82"/>
-      <c r="V19" s="315"/>
-      <c r="W19" s="316"/>
-      <c r="X19" s="316"/>
-      <c r="Y19" s="316"/>
-      <c r="Z19" s="316"/>
-      <c r="AA19" s="316"/>
-      <c r="AB19" s="316"/>
-      <c r="AC19" s="316"/>
-      <c r="AD19" s="316"/>
-      <c r="AE19" s="316"/>
-      <c r="AF19" s="316"/>
-      <c r="AG19" s="316"/>
-      <c r="AH19" s="316"/>
-      <c r="AI19" s="316"/>
-      <c r="AJ19" s="316"/>
-      <c r="AK19" s="316"/>
-      <c r="AL19" s="316"/>
-      <c r="AM19" s="316"/>
-      <c r="AN19" s="316"/>
-      <c r="AO19" s="316"/>
-      <c r="AP19" s="316"/>
-      <c r="AQ19" s="316"/>
-      <c r="AR19" s="316"/>
-      <c r="AS19" s="292"/>
+      <c r="V19" s="292"/>
+      <c r="W19" s="293"/>
+      <c r="X19" s="293"/>
+      <c r="Y19" s="293"/>
+      <c r="Z19" s="293"/>
+      <c r="AA19" s="293"/>
+      <c r="AB19" s="293"/>
+      <c r="AC19" s="293"/>
+      <c r="AD19" s="293"/>
+      <c r="AE19" s="293"/>
+      <c r="AF19" s="293"/>
+      <c r="AG19" s="293"/>
+      <c r="AH19" s="293"/>
+      <c r="AI19" s="293"/>
+      <c r="AJ19" s="293"/>
+      <c r="AK19" s="293"/>
+      <c r="AL19" s="293"/>
+      <c r="AM19" s="293"/>
+      <c r="AN19" s="293"/>
+      <c r="AO19" s="293"/>
+      <c r="AP19" s="293"/>
+      <c r="AQ19" s="293"/>
+      <c r="AR19" s="293"/>
+      <c r="AS19" s="294"/>
       <c r="AT19" s="82"/>
     </row>
     <row r="20" spans="1:46" ht="16.5" customHeight="1">
@@ -44696,7 +44697,7 @@
       <c r="S21" s="82"/>
       <c r="T21" s="82"/>
       <c r="U21" s="82"/>
-      <c r="V21" s="294" t="s">
+      <c r="V21" s="286" t="s">
         <v>109</v>
       </c>
       <c r="W21" s="248"/>
@@ -44726,29 +44727,29 @@
     </row>
     <row r="22" spans="1:46" ht="16.5" customHeight="1">
       <c r="A22" s="82"/>
-      <c r="B22" s="283" t="s">
+      <c r="B22" s="310" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="283"/>
-      <c r="D22" s="283"/>
-      <c r="E22" s="283"/>
-      <c r="F22" s="283"/>
-      <c r="G22" s="283"/>
-      <c r="H22" s="283"/>
-      <c r="I22" s="283"/>
-      <c r="J22" s="283"/>
-      <c r="K22" s="283"/>
-      <c r="L22" s="283"/>
-      <c r="M22" s="283"/>
-      <c r="N22" s="283"/>
-      <c r="O22" s="283"/>
+      <c r="C22" s="310"/>
+      <c r="D22" s="310"/>
+      <c r="E22" s="310"/>
+      <c r="F22" s="310"/>
+      <c r="G22" s="310"/>
+      <c r="H22" s="310"/>
+      <c r="I22" s="310"/>
+      <c r="J22" s="310"/>
+      <c r="K22" s="310"/>
+      <c r="L22" s="310"/>
+      <c r="M22" s="310"/>
+      <c r="N22" s="310"/>
+      <c r="O22" s="310"/>
       <c r="P22" s="201"/>
       <c r="Q22" s="201"/>
       <c r="R22" s="82"/>
       <c r="S22" s="82"/>
       <c r="T22" s="82"/>
       <c r="U22" s="82"/>
-      <c r="V22" s="285" t="s">
+      <c r="V22" s="283" t="s">
         <v>111</v>
       </c>
       <c r="W22" s="248"/>
@@ -44763,14 +44764,14 @@
       <c r="AF22" s="248"/>
       <c r="AG22" s="248"/>
       <c r="AH22" s="249"/>
-      <c r="AI22" s="285" t="s">
+      <c r="AI22" s="283" t="s">
         <v>99</v>
       </c>
       <c r="AJ22" s="248"/>
       <c r="AK22" s="248"/>
       <c r="AL22" s="248"/>
       <c r="AM22" s="249"/>
-      <c r="AN22" s="285" t="s">
+      <c r="AN22" s="283" t="s">
         <v>113</v>
       </c>
       <c r="AO22" s="248"/>
@@ -44818,15 +44819,15 @@
       <c r="M23" s="203" t="s">
         <v>95</v>
       </c>
-      <c r="N23" s="307" t="s">
+      <c r="N23" s="306" t="s">
         <v>47</v>
       </c>
-      <c r="O23" s="308"/>
+      <c r="O23" s="307"/>
       <c r="R23" s="82"/>
       <c r="S23" s="82"/>
       <c r="T23" s="82"/>
       <c r="U23" s="82"/>
-      <c r="V23" s="284" t="s">
+      <c r="V23" s="295" t="s">
         <v>114</v>
       </c>
       <c r="W23" s="248"/>
@@ -44841,14 +44842,14 @@
       <c r="AF23" s="248"/>
       <c r="AG23" s="248"/>
       <c r="AH23" s="249"/>
-      <c r="AI23" s="284">
+      <c r="AI23" s="295">
         <v>22</v>
       </c>
       <c r="AJ23" s="248"/>
       <c r="AK23" s="248"/>
       <c r="AL23" s="248"/>
       <c r="AM23" s="249"/>
-      <c r="AN23" s="295">
+      <c r="AN23" s="284">
         <f>AI23/R33</f>
         <v>1</v>
       </c>
@@ -44909,16 +44910,16 @@
         <f>GradeSheet!$H$38</f>
         <v>0</v>
       </c>
-      <c r="N24" s="291">
+      <c r="N24" s="316">
         <f>SUM(B24:M24)</f>
         <v>14</v>
       </c>
-      <c r="O24" s="292"/>
+      <c r="O24" s="294"/>
       <c r="R24" s="82"/>
       <c r="S24" s="82"/>
       <c r="T24" s="82"/>
       <c r="U24" s="82"/>
-      <c r="V24" s="284" t="s">
+      <c r="V24" s="295" t="s">
         <v>115</v>
       </c>
       <c r="W24" s="248"/>
@@ -44933,14 +44934,14 @@
       <c r="AF24" s="248"/>
       <c r="AG24" s="248"/>
       <c r="AH24" s="249"/>
-      <c r="AI24" s="284">
+      <c r="AI24" s="295">
         <v>0</v>
       </c>
       <c r="AJ24" s="248"/>
       <c r="AK24" s="248"/>
       <c r="AL24" s="248"/>
       <c r="AM24" s="249"/>
-      <c r="AN24" s="295">
+      <c r="AN24" s="284">
         <f>AI24/R33</f>
         <v>0</v>
       </c>
@@ -45001,7 +45002,7 @@
         <f>M24/GradeSheet!$H$39</f>
         <v>0</v>
       </c>
-      <c r="N25" s="293">
+      <c r="N25" s="317">
         <f>SUM(B25:M25)</f>
         <v>1</v>
       </c>
@@ -45010,7 +45011,7 @@
       <c r="S25" s="82"/>
       <c r="T25" s="82"/>
       <c r="U25" s="82"/>
-      <c r="V25" s="284" t="s">
+      <c r="V25" s="295" t="s">
         <v>46</v>
       </c>
       <c r="W25" s="248"/>
@@ -45025,14 +45026,14 @@
       <c r="AF25" s="248"/>
       <c r="AG25" s="248"/>
       <c r="AH25" s="249"/>
-      <c r="AI25" s="284">
+      <c r="AI25" s="295">
         <v>0</v>
       </c>
       <c r="AJ25" s="248"/>
       <c r="AK25" s="248"/>
       <c r="AL25" s="248"/>
       <c r="AM25" s="249"/>
-      <c r="AN25" s="295">
+      <c r="AN25" s="284">
         <f>AI25/R33</f>
         <v>0</v>
       </c>
@@ -45065,7 +45066,7 @@
       <c r="S26" s="82"/>
       <c r="T26" s="82"/>
       <c r="U26" s="82"/>
-      <c r="V26" s="284" t="s">
+      <c r="V26" s="295" t="s">
         <v>120</v>
       </c>
       <c r="W26" s="248"/>
@@ -45080,14 +45081,14 @@
       <c r="AF26" s="248"/>
       <c r="AG26" s="248"/>
       <c r="AH26" s="249"/>
-      <c r="AI26" s="284">
+      <c r="AI26" s="295">
         <v>22</v>
       </c>
       <c r="AJ26" s="248"/>
       <c r="AK26" s="248"/>
       <c r="AL26" s="248"/>
       <c r="AM26" s="249"/>
-      <c r="AN26" s="295">
+      <c r="AN26" s="284">
         <f>AI26/R33</f>
         <v>1</v>
       </c>
@@ -45122,7 +45123,7 @@
       <c r="S27" s="82"/>
       <c r="T27" s="82"/>
       <c r="U27" s="82"/>
-      <c r="V27" s="284"/>
+      <c r="V27" s="295"/>
       <c r="W27" s="248"/>
       <c r="X27" s="248"/>
       <c r="Y27" s="248"/>
@@ -45135,12 +45136,12 @@
       <c r="AF27" s="248"/>
       <c r="AG27" s="248"/>
       <c r="AH27" s="249"/>
-      <c r="AI27" s="284"/>
+      <c r="AI27" s="295"/>
       <c r="AJ27" s="248"/>
       <c r="AK27" s="248"/>
       <c r="AL27" s="248"/>
       <c r="AM27" s="249"/>
-      <c r="AN27" s="295"/>
+      <c r="AN27" s="284"/>
       <c r="AO27" s="248"/>
       <c r="AP27" s="248"/>
       <c r="AQ27" s="248"/>
@@ -45170,7 +45171,7 @@
       <c r="S28" s="82"/>
       <c r="T28" s="82"/>
       <c r="U28" s="82"/>
-      <c r="V28" s="309"/>
+      <c r="V28" s="285"/>
       <c r="W28" s="254"/>
       <c r="X28" s="254"/>
       <c r="Y28" s="254"/>
@@ -45183,12 +45184,12 @@
       <c r="AF28" s="254"/>
       <c r="AG28" s="254"/>
       <c r="AH28" s="254"/>
-      <c r="AI28" s="309"/>
+      <c r="AI28" s="285"/>
       <c r="AJ28" s="254"/>
       <c r="AK28" s="254"/>
       <c r="AL28" s="254"/>
       <c r="AM28" s="254"/>
-      <c r="AN28" s="309"/>
+      <c r="AN28" s="285"/>
       <c r="AO28" s="254"/>
       <c r="AP28" s="254"/>
       <c r="AQ28" s="254"/>
@@ -45198,7 +45199,7 @@
     </row>
     <row r="29" spans="1:46" ht="16.5" customHeight="1">
       <c r="A29" s="82"/>
-      <c r="B29" s="285"/>
+      <c r="B29" s="283"/>
       <c r="C29" s="248"/>
       <c r="D29" s="248"/>
       <c r="E29" s="248"/>
@@ -45210,7 +45211,7 @@
         <v>123</v>
       </c>
       <c r="I29" s="82"/>
-      <c r="J29" s="285"/>
+      <c r="J29" s="283"/>
       <c r="K29" s="248"/>
       <c r="L29" s="248"/>
       <c r="M29" s="248"/>
@@ -45226,7 +45227,7 @@
       </c>
       <c r="T29" s="82"/>
       <c r="U29" s="82"/>
-      <c r="V29" s="309"/>
+      <c r="V29" s="285"/>
       <c r="W29" s="254"/>
       <c r="X29" s="254"/>
       <c r="Y29" s="254"/>
@@ -45239,12 +45240,12 @@
       <c r="AF29" s="254"/>
       <c r="AG29" s="254"/>
       <c r="AH29" s="254"/>
-      <c r="AI29" s="309"/>
+      <c r="AI29" s="285"/>
       <c r="AJ29" s="254"/>
       <c r="AK29" s="254"/>
       <c r="AL29" s="254"/>
       <c r="AM29" s="254"/>
-      <c r="AN29" s="309"/>
+      <c r="AN29" s="285"/>
       <c r="AO29" s="254"/>
       <c r="AP29" s="254"/>
       <c r="AQ29" s="254"/>
@@ -45254,7 +45255,7 @@
     </row>
     <row r="30" spans="1:46" ht="16.5" customHeight="1">
       <c r="A30" s="82"/>
-      <c r="B30" s="285" t="s">
+      <c r="B30" s="283" t="s">
         <v>125</v>
       </c>
       <c r="C30" s="248"/>
@@ -45270,7 +45271,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="82"/>
-      <c r="J30" s="285" t="s">
+      <c r="J30" s="283" t="s">
         <v>126</v>
       </c>
       <c r="K30" s="248"/>
@@ -45289,7 +45290,7 @@
       </c>
       <c r="T30" s="82"/>
       <c r="U30" s="82"/>
-      <c r="V30" s="294" t="s">
+      <c r="V30" s="286" t="s">
         <v>128</v>
       </c>
       <c r="W30" s="248"/>
@@ -45304,14 +45305,14 @@
       <c r="AF30" s="248"/>
       <c r="AG30" s="248"/>
       <c r="AH30" s="249"/>
-      <c r="AI30" s="285" t="s">
+      <c r="AI30" s="283" t="s">
         <v>99</v>
       </c>
       <c r="AJ30" s="248"/>
       <c r="AK30" s="248"/>
       <c r="AL30" s="248"/>
       <c r="AM30" s="249"/>
-      <c r="AN30" s="285" t="s">
+      <c r="AN30" s="283" t="s">
         <v>113</v>
       </c>
       <c r="AO30" s="248"/>
@@ -45323,7 +45324,7 @@
     </row>
     <row r="31" spans="1:46" ht="16.5" customHeight="1">
       <c r="A31" s="82"/>
-      <c r="B31" s="285" t="s">
+      <c r="B31" s="283" t="s">
         <v>129</v>
       </c>
       <c r="C31" s="248"/>
@@ -45339,7 +45340,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="82"/>
-      <c r="J31" s="285" t="s">
+      <c r="J31" s="283" t="s">
         <v>134</v>
       </c>
       <c r="K31" s="248"/>
@@ -45358,7 +45359,7 @@
       </c>
       <c r="T31" s="82"/>
       <c r="U31" s="82"/>
-      <c r="V31" s="284" t="s">
+      <c r="V31" s="295" t="s">
         <v>120</v>
       </c>
       <c r="W31" s="248"/>
@@ -45373,14 +45374,14 @@
       <c r="AF31" s="248"/>
       <c r="AG31" s="248"/>
       <c r="AH31" s="249"/>
-      <c r="AI31" s="284">
+      <c r="AI31" s="295">
         <v>22</v>
       </c>
       <c r="AJ31" s="248"/>
       <c r="AK31" s="248"/>
       <c r="AL31" s="248"/>
       <c r="AM31" s="249"/>
-      <c r="AN31" s="295">
+      <c r="AN31" s="284">
         <f>AI31/R33</f>
         <v>1</v>
       </c>
@@ -45393,7 +45394,7 @@
     </row>
     <row r="32" spans="1:46" ht="16.5" customHeight="1">
       <c r="A32" s="114"/>
-      <c r="B32" s="285" t="s">
+      <c r="B32" s="283" t="s">
         <v>135</v>
       </c>
       <c r="C32" s="248"/>
@@ -45409,7 +45410,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="82"/>
-      <c r="J32" s="285" t="s">
+      <c r="J32" s="283" t="s">
         <v>136</v>
       </c>
       <c r="K32" s="248"/>
@@ -45428,7 +45429,7 @@
       </c>
       <c r="T32" s="82"/>
       <c r="U32" s="82"/>
-      <c r="V32" s="284" t="s">
+      <c r="V32" s="295" t="s">
         <v>115</v>
       </c>
       <c r="W32" s="248"/>
@@ -45443,14 +45444,14 @@
       <c r="AF32" s="248"/>
       <c r="AG32" s="248"/>
       <c r="AH32" s="249"/>
-      <c r="AI32" s="284">
+      <c r="AI32" s="295">
         <v>0</v>
       </c>
       <c r="AJ32" s="248"/>
       <c r="AK32" s="248"/>
       <c r="AL32" s="248"/>
       <c r="AM32" s="249"/>
-      <c r="AN32" s="295">
+      <c r="AN32" s="284">
         <f>AI32/R33</f>
         <v>0</v>
       </c>
@@ -45463,7 +45464,7 @@
     </row>
     <row r="33" spans="1:46" ht="17.25" customHeight="1">
       <c r="A33" s="82"/>
-      <c r="B33" s="285" t="s">
+      <c r="B33" s="283" t="s">
         <v>137</v>
       </c>
       <c r="C33" s="248"/>
@@ -45479,26 +45480,26 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="I33" s="82"/>
-      <c r="J33" s="310" t="s">
+      <c r="J33" s="287" t="s">
         <v>138</v>
       </c>
-      <c r="K33" s="311"/>
-      <c r="L33" s="311"/>
-      <c r="M33" s="311"/>
-      <c r="N33" s="311"/>
-      <c r="O33" s="311"/>
-      <c r="P33" s="311"/>
-      <c r="Q33" s="312"/>
-      <c r="R33" s="290">
+      <c r="K33" s="288"/>
+      <c r="L33" s="288"/>
+      <c r="M33" s="288"/>
+      <c r="N33" s="288"/>
+      <c r="O33" s="288"/>
+      <c r="P33" s="288"/>
+      <c r="Q33" s="289"/>
+      <c r="R33" s="315">
         <v>22</v>
       </c>
-      <c r="S33" s="287">
+      <c r="S33" s="312">
         <f>R33/R30</f>
         <v>0.91666666666666663</v>
       </c>
       <c r="T33" s="82"/>
       <c r="U33" s="82"/>
-      <c r="V33" s="285"/>
+      <c r="V33" s="283"/>
       <c r="W33" s="248"/>
       <c r="X33" s="248"/>
       <c r="Y33" s="248"/>
@@ -45511,12 +45512,12 @@
       <c r="AF33" s="248"/>
       <c r="AG33" s="248"/>
       <c r="AH33" s="249"/>
-      <c r="AI33" s="285"/>
+      <c r="AI33" s="283"/>
       <c r="AJ33" s="248"/>
       <c r="AK33" s="248"/>
       <c r="AL33" s="248"/>
       <c r="AM33" s="249"/>
-      <c r="AN33" s="285"/>
+      <c r="AN33" s="283"/>
       <c r="AO33" s="248"/>
       <c r="AP33" s="248"/>
       <c r="AQ33" s="248"/>
@@ -45534,16 +45535,16 @@
       <c r="G34" s="84"/>
       <c r="H34" s="84"/>
       <c r="I34" s="82"/>
-      <c r="J34" s="313"/>
+      <c r="J34" s="290"/>
       <c r="K34" s="254"/>
       <c r="L34" s="254"/>
       <c r="M34" s="254"/>
       <c r="N34" s="254"/>
       <c r="O34" s="254"/>
       <c r="P34" s="254"/>
-      <c r="Q34" s="314"/>
-      <c r="R34" s="288"/>
-      <c r="S34" s="288"/>
+      <c r="Q34" s="291"/>
+      <c r="R34" s="313"/>
+      <c r="S34" s="313"/>
       <c r="T34" s="82"/>
       <c r="U34" s="82"/>
       <c r="V34" s="82"/>
@@ -45582,16 +45583,16 @@
       <c r="G35" s="84"/>
       <c r="H35" s="84"/>
       <c r="I35" s="82"/>
-      <c r="J35" s="315"/>
-      <c r="K35" s="316"/>
-      <c r="L35" s="316"/>
-      <c r="M35" s="316"/>
-      <c r="N35" s="316"/>
-      <c r="O35" s="316"/>
-      <c r="P35" s="316"/>
-      <c r="Q35" s="292"/>
-      <c r="R35" s="289"/>
-      <c r="S35" s="289"/>
+      <c r="J35" s="292"/>
+      <c r="K35" s="293"/>
+      <c r="L35" s="293"/>
+      <c r="M35" s="293"/>
+      <c r="N35" s="293"/>
+      <c r="O35" s="293"/>
+      <c r="P35" s="293"/>
+      <c r="Q35" s="294"/>
+      <c r="R35" s="314"/>
+      <c r="S35" s="314"/>
       <c r="T35" s="82"/>
       <c r="U35" s="82"/>
       <c r="V35" s="82"/>
@@ -45670,7 +45671,7 @@
     </row>
     <row r="37" spans="1:46" ht="16.5" customHeight="1">
       <c r="A37" s="82"/>
-      <c r="B37" s="285" t="s">
+      <c r="B37" s="283" t="s">
         <v>139</v>
       </c>
       <c r="C37" s="248"/>
@@ -45680,7 +45681,7 @@
       <c r="G37" s="249"/>
       <c r="H37" s="82"/>
       <c r="I37" s="82"/>
-      <c r="J37" s="285"/>
+      <c r="J37" s="283"/>
       <c r="K37" s="248"/>
       <c r="L37" s="248"/>
       <c r="M37" s="248"/>
@@ -45688,13 +45689,13 @@
       <c r="O37" s="248"/>
       <c r="P37" s="248"/>
       <c r="Q37" s="249"/>
-      <c r="R37" s="286" t="s">
+      <c r="R37" s="311" t="s">
         <v>124</v>
       </c>
       <c r="S37" s="249"/>
       <c r="T37" s="82"/>
       <c r="U37" s="82"/>
-      <c r="V37" s="294" t="s">
+      <c r="V37" s="286" t="s">
         <v>140</v>
       </c>
       <c r="W37" s="248"/>
@@ -45709,14 +45710,14 @@
       <c r="AF37" s="248"/>
       <c r="AG37" s="248"/>
       <c r="AH37" s="249"/>
-      <c r="AI37" s="285" t="s">
+      <c r="AI37" s="283" t="s">
         <v>99</v>
       </c>
       <c r="AJ37" s="248"/>
       <c r="AK37" s="248"/>
       <c r="AL37" s="248"/>
       <c r="AM37" s="249"/>
-      <c r="AN37" s="285" t="s">
+      <c r="AN37" s="283" t="s">
         <v>113</v>
       </c>
       <c r="AO37" s="248"/>
@@ -45728,7 +45729,7 @@
     </row>
     <row r="38" spans="1:46" ht="16.5" customHeight="1">
       <c r="A38" s="82"/>
-      <c r="B38" s="285" t="s">
+      <c r="B38" s="283" t="s">
         <v>141</v>
       </c>
       <c r="C38" s="248"/>
@@ -45738,7 +45739,7 @@
       <c r="G38" s="105"/>
       <c r="H38" s="82"/>
       <c r="I38" s="82"/>
-      <c r="J38" s="285" t="s">
+      <c r="J38" s="283" t="s">
         <v>142</v>
       </c>
       <c r="K38" s="248"/>
@@ -45748,13 +45749,13 @@
       <c r="O38" s="248"/>
       <c r="P38" s="248"/>
       <c r="Q38" s="249"/>
-      <c r="R38" s="284" t="s">
+      <c r="R38" s="295" t="s">
         <v>143</v>
       </c>
       <c r="S38" s="249"/>
       <c r="T38" s="82"/>
       <c r="U38" s="82"/>
-      <c r="V38" s="284" t="s">
+      <c r="V38" s="295" t="s">
         <v>144</v>
       </c>
       <c r="W38" s="248"/>
@@ -45769,14 +45770,14 @@
       <c r="AF38" s="248"/>
       <c r="AG38" s="248"/>
       <c r="AH38" s="249"/>
-      <c r="AI38" s="284">
+      <c r="AI38" s="295">
         <v>22</v>
       </c>
       <c r="AJ38" s="248"/>
       <c r="AK38" s="248"/>
       <c r="AL38" s="248"/>
       <c r="AM38" s="249"/>
-      <c r="AN38" s="295">
+      <c r="AN38" s="284">
         <f>AI38/R33</f>
         <v>1</v>
       </c>
@@ -45789,7 +45790,7 @@
     </row>
     <row r="39" spans="1:46" ht="16.5" customHeight="1">
       <c r="A39" s="82"/>
-      <c r="B39" s="285" t="s">
+      <c r="B39" s="283" t="s">
         <v>145</v>
       </c>
       <c r="C39" s="248"/>
@@ -45799,7 +45800,7 @@
       <c r="G39" s="105"/>
       <c r="H39" s="82"/>
       <c r="I39" s="82"/>
-      <c r="J39" s="285" t="s">
+      <c r="J39" s="283" t="s">
         <v>146</v>
       </c>
       <c r="K39" s="248"/>
@@ -45809,13 +45810,13 @@
       <c r="O39" s="248"/>
       <c r="P39" s="248"/>
       <c r="Q39" s="249"/>
-      <c r="R39" s="284" t="s">
+      <c r="R39" s="295" t="s">
         <v>143</v>
       </c>
       <c r="S39" s="249"/>
       <c r="T39" s="82"/>
       <c r="U39" s="82"/>
-      <c r="V39" s="284" t="s">
+      <c r="V39" s="295" t="s">
         <v>147</v>
       </c>
       <c r="W39" s="248"/>
@@ -45830,14 +45831,14 @@
       <c r="AF39" s="248"/>
       <c r="AG39" s="248"/>
       <c r="AH39" s="249"/>
-      <c r="AI39" s="284">
+      <c r="AI39" s="295">
         <v>0</v>
       </c>
       <c r="AJ39" s="248"/>
       <c r="AK39" s="248"/>
       <c r="AL39" s="248"/>
       <c r="AM39" s="249"/>
-      <c r="AN39" s="295">
+      <c r="AN39" s="284">
         <f>AI39/R33</f>
         <v>0</v>
       </c>
@@ -45870,7 +45871,7 @@
       <c r="S40" s="82"/>
       <c r="T40" s="82"/>
       <c r="U40" s="82"/>
-      <c r="V40" s="284" t="s">
+      <c r="V40" s="295" t="s">
         <v>148</v>
       </c>
       <c r="W40" s="248"/>
@@ -45885,14 +45886,14 @@
       <c r="AF40" s="248"/>
       <c r="AG40" s="248"/>
       <c r="AH40" s="249"/>
-      <c r="AI40" s="284">
+      <c r="AI40" s="295">
         <v>22</v>
       </c>
       <c r="AJ40" s="248"/>
       <c r="AK40" s="248"/>
       <c r="AL40" s="248"/>
       <c r="AM40" s="249"/>
-      <c r="AN40" s="295">
+      <c r="AN40" s="284">
         <f>AI40/R33</f>
         <v>1</v>
       </c>
@@ -45925,7 +45926,7 @@
       <c r="S41" s="82"/>
       <c r="T41" s="82"/>
       <c r="U41" s="82"/>
-      <c r="V41" s="284" t="s">
+      <c r="V41" s="295" t="s">
         <v>149</v>
       </c>
       <c r="W41" s="248"/>
@@ -45940,14 +45941,14 @@
       <c r="AF41" s="248"/>
       <c r="AG41" s="248"/>
       <c r="AH41" s="249"/>
-      <c r="AI41" s="284">
+      <c r="AI41" s="295">
         <v>0</v>
       </c>
       <c r="AJ41" s="248"/>
       <c r="AK41" s="248"/>
       <c r="AL41" s="248"/>
       <c r="AM41" s="249"/>
-      <c r="AN41" s="295">
+      <c r="AN41" s="284">
         <f>AI41/R33</f>
         <v>0</v>
       </c>
@@ -45980,7 +45981,7 @@
       <c r="S42" s="82"/>
       <c r="T42" s="82"/>
       <c r="U42" s="82"/>
-      <c r="V42" s="284"/>
+      <c r="V42" s="295"/>
       <c r="W42" s="248"/>
       <c r="X42" s="248"/>
       <c r="Y42" s="248"/>
@@ -45993,12 +45994,12 @@
       <c r="AF42" s="248"/>
       <c r="AG42" s="248"/>
       <c r="AH42" s="249"/>
-      <c r="AI42" s="284"/>
+      <c r="AI42" s="295"/>
       <c r="AJ42" s="248"/>
       <c r="AK42" s="248"/>
       <c r="AL42" s="248"/>
       <c r="AM42" s="249"/>
-      <c r="AN42" s="295"/>
+      <c r="AN42" s="284"/>
       <c r="AO42" s="248"/>
       <c r="AP42" s="248"/>
       <c r="AQ42" s="248"/>
@@ -46394,12 +46395,12 @@
     </row>
     <row r="51" spans="1:46" ht="16.5" customHeight="1">
       <c r="A51" s="82"/>
-      <c r="B51" s="303" t="s">
+      <c r="B51" s="300" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="248"/>
       <c r="D51" s="249"/>
-      <c r="E51" s="305" t="str">
+      <c r="E51" s="302" t="str">
         <f>GradeSheet!$H$2</f>
         <v>CSE 208</v>
       </c>
@@ -46414,7 +46415,7 @@
       <c r="N51" s="248"/>
       <c r="O51" s="248"/>
       <c r="P51" s="249"/>
-      <c r="Q51" s="303" t="str">
+      <c r="Q51" s="300" t="str">
         <f>CONCATENATE("Section ", GradeSheet!$L$2,)</f>
         <v>Section 1</v>
       </c>
@@ -46450,12 +46451,12 @@
     </row>
     <row r="52" spans="1:46" ht="16.5" customHeight="1">
       <c r="A52" s="82"/>
-      <c r="B52" s="302" t="s">
+      <c r="B52" s="301" t="s">
         <v>52</v>
       </c>
       <c r="C52" s="248"/>
       <c r="D52" s="249"/>
-      <c r="E52" s="304" t="str">
+      <c r="E52" s="299" t="str">
         <f>GradeSheet!$H$3</f>
         <v>Data Structure Lab</v>
       </c>
@@ -46470,7 +46471,7 @@
       <c r="N52" s="248"/>
       <c r="O52" s="248"/>
       <c r="P52" s="249"/>
-      <c r="Q52" s="302" t="str">
+      <c r="Q52" s="301" t="str">
         <f>CONCATENATE(GradeSheet!$H$39," students")</f>
         <v>14 students</v>
       </c>
@@ -46506,12 +46507,12 @@
     </row>
     <row r="53" spans="1:46" ht="16.5" customHeight="1">
       <c r="A53" s="82"/>
-      <c r="B53" s="301" t="s">
+      <c r="B53" s="305" t="s">
         <v>54</v>
       </c>
       <c r="C53" s="248"/>
       <c r="D53" s="249"/>
-      <c r="E53" s="300">
+      <c r="E53" s="304">
         <f>GradeSheet!$H$4</f>
         <v>3</v>
       </c>
@@ -46526,7 +46527,7 @@
       <c r="N53" s="248"/>
       <c r="O53" s="248"/>
       <c r="P53" s="249"/>
-      <c r="Q53" s="300" t="str">
+      <c r="Q53" s="304" t="str">
         <f>GradeSheet!$L$3</f>
         <v>Fall 2019</v>
       </c>
@@ -46709,7 +46710,7 @@
       <c r="B57" s="82"/>
       <c r="C57" s="82"/>
       <c r="D57" s="82"/>
-      <c r="E57" s="298" t="s">
+      <c r="E57" s="308" t="s">
         <v>151</v>
       </c>
       <c r="F57" s="248"/>
@@ -46759,7 +46760,7 @@
       <c r="B58" s="82"/>
       <c r="C58" s="82"/>
       <c r="D58" s="82"/>
-      <c r="E58" s="299"/>
+      <c r="E58" s="309"/>
       <c r="F58" s="248"/>
       <c r="G58" s="249"/>
       <c r="H58" s="88" t="s">
@@ -46819,7 +46820,7 @@
       <c r="B59" s="82"/>
       <c r="C59" s="82"/>
       <c r="D59" s="82"/>
-      <c r="E59" s="297" t="s">
+      <c r="E59" s="298" t="s">
         <v>116</v>
       </c>
       <c r="F59" s="248"/>
@@ -46887,7 +46888,7 @@
       <c r="B60" s="82"/>
       <c r="C60" s="82"/>
       <c r="D60" s="82"/>
-      <c r="E60" s="297" t="s">
+      <c r="E60" s="298" t="s">
         <v>152</v>
       </c>
       <c r="F60" s="248"/>
@@ -57292,25 +57293,94 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="131">
-    <mergeCell ref="V33:AH33"/>
-    <mergeCell ref="AN32:AS32"/>
-    <mergeCell ref="V29:AH29"/>
-    <mergeCell ref="V30:AH30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="J32:Q32"/>
-    <mergeCell ref="J31:Q31"/>
-    <mergeCell ref="J33:Q35"/>
-    <mergeCell ref="AN28:AS28"/>
-    <mergeCell ref="AI27:AM27"/>
-    <mergeCell ref="AI31:AM31"/>
-    <mergeCell ref="AN31:AS31"/>
-    <mergeCell ref="AI30:AM30"/>
-    <mergeCell ref="AN30:AS30"/>
-    <mergeCell ref="AI29:AM29"/>
-    <mergeCell ref="AN29:AS29"/>
-    <mergeCell ref="AN33:AS33"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="AI42:AM42"/>
+    <mergeCell ref="AI41:AM41"/>
+    <mergeCell ref="AI37:AM37"/>
+    <mergeCell ref="AI38:AM38"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="AI33:AM33"/>
+    <mergeCell ref="AI32:AM32"/>
+    <mergeCell ref="V31:AH31"/>
+    <mergeCell ref="V32:AH32"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="S33:S35"/>
+    <mergeCell ref="R33:R35"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="J37:Q37"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="V40:AH40"/>
+    <mergeCell ref="V41:AH41"/>
+    <mergeCell ref="V42:AH42"/>
+    <mergeCell ref="V39:AH39"/>
+    <mergeCell ref="V38:AH38"/>
+    <mergeCell ref="V37:AH37"/>
+    <mergeCell ref="AN41:AS41"/>
+    <mergeCell ref="AN40:AS40"/>
+    <mergeCell ref="AI40:AM40"/>
+    <mergeCell ref="AI39:AM39"/>
+    <mergeCell ref="V2:AP2"/>
+    <mergeCell ref="V11:AH11"/>
+    <mergeCell ref="V12:AH12"/>
+    <mergeCell ref="V23:AH23"/>
+    <mergeCell ref="V22:AH22"/>
+    <mergeCell ref="AI22:AM22"/>
+    <mergeCell ref="V21:AS21"/>
+    <mergeCell ref="V6:AH6"/>
+    <mergeCell ref="AI6:AP6"/>
+    <mergeCell ref="AI11:AP11"/>
+    <mergeCell ref="AI12:AP12"/>
+    <mergeCell ref="AI9:AP9"/>
+    <mergeCell ref="AI10:AP10"/>
+    <mergeCell ref="V9:AH9"/>
+    <mergeCell ref="V10:AH10"/>
+    <mergeCell ref="V14:AP14"/>
+    <mergeCell ref="AI7:AP7"/>
+    <mergeCell ref="AI8:AP8"/>
+    <mergeCell ref="V7:AH7"/>
+    <mergeCell ref="V8:AH8"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="J39:Q39"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="E57:M57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E53:P53"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="Q52:S52"/>
+    <mergeCell ref="Q51:S51"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E52:P52"/>
+    <mergeCell ref="E51:P51"/>
+    <mergeCell ref="J38:Q38"/>
+    <mergeCell ref="AN38:AS38"/>
+    <mergeCell ref="AN39:AS39"/>
+    <mergeCell ref="AN37:AS37"/>
+    <mergeCell ref="AN42:AS42"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E3:P3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="E2:P2"/>
+    <mergeCell ref="AI3:AP3"/>
+    <mergeCell ref="AI4:AP4"/>
+    <mergeCell ref="AI5:AP5"/>
+    <mergeCell ref="V5:AH5"/>
+    <mergeCell ref="E4:P4"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="V3:AH3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="V4:AH4"/>
+    <mergeCell ref="V24:AH24"/>
+    <mergeCell ref="V25:AH25"/>
+    <mergeCell ref="AN24:AS24"/>
+    <mergeCell ref="N23:O23"/>
     <mergeCell ref="V26:AH26"/>
     <mergeCell ref="V27:AH27"/>
     <mergeCell ref="J30:Q30"/>
@@ -57335,94 +57405,25 @@
     <mergeCell ref="AN26:AS26"/>
     <mergeCell ref="AN27:AS27"/>
     <mergeCell ref="AI28:AM28"/>
-    <mergeCell ref="AN38:AS38"/>
-    <mergeCell ref="AN39:AS39"/>
-    <mergeCell ref="AN37:AS37"/>
-    <mergeCell ref="AN42:AS42"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E3:P3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="E2:P2"/>
-    <mergeCell ref="AI3:AP3"/>
-    <mergeCell ref="AI4:AP4"/>
-    <mergeCell ref="AI5:AP5"/>
-    <mergeCell ref="V5:AH5"/>
-    <mergeCell ref="E4:P4"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="V3:AH3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="V4:AH4"/>
-    <mergeCell ref="V24:AH24"/>
-    <mergeCell ref="V25:AH25"/>
-    <mergeCell ref="AN24:AS24"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="J39:Q39"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="E57:M57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E53:P53"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="Q52:S52"/>
-    <mergeCell ref="Q51:S51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="E52:P52"/>
-    <mergeCell ref="E51:P51"/>
-    <mergeCell ref="J38:Q38"/>
-    <mergeCell ref="AN41:AS41"/>
-    <mergeCell ref="AN40:AS40"/>
-    <mergeCell ref="AI40:AM40"/>
-    <mergeCell ref="AI39:AM39"/>
-    <mergeCell ref="V2:AP2"/>
-    <mergeCell ref="V11:AH11"/>
-    <mergeCell ref="V12:AH12"/>
-    <mergeCell ref="V23:AH23"/>
-    <mergeCell ref="V22:AH22"/>
-    <mergeCell ref="AI22:AM22"/>
-    <mergeCell ref="V21:AS21"/>
-    <mergeCell ref="V6:AH6"/>
-    <mergeCell ref="AI6:AP6"/>
-    <mergeCell ref="AI11:AP11"/>
-    <mergeCell ref="AI12:AP12"/>
-    <mergeCell ref="AI9:AP9"/>
-    <mergeCell ref="AI10:AP10"/>
-    <mergeCell ref="V9:AH9"/>
-    <mergeCell ref="V10:AH10"/>
-    <mergeCell ref="V14:AP14"/>
-    <mergeCell ref="AI7:AP7"/>
-    <mergeCell ref="AI8:AP8"/>
-    <mergeCell ref="V7:AH7"/>
-    <mergeCell ref="V8:AH8"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="AI42:AM42"/>
-    <mergeCell ref="AI41:AM41"/>
-    <mergeCell ref="AI37:AM37"/>
-    <mergeCell ref="AI38:AM38"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="AI33:AM33"/>
-    <mergeCell ref="AI32:AM32"/>
-    <mergeCell ref="V31:AH31"/>
-    <mergeCell ref="V32:AH32"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="S33:S35"/>
-    <mergeCell ref="R33:R35"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="J37:Q37"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="V40:AH40"/>
-    <mergeCell ref="V41:AH41"/>
-    <mergeCell ref="V42:AH42"/>
-    <mergeCell ref="V39:AH39"/>
-    <mergeCell ref="V38:AH38"/>
-    <mergeCell ref="V37:AH37"/>
+    <mergeCell ref="AN28:AS28"/>
+    <mergeCell ref="AI27:AM27"/>
+    <mergeCell ref="AI31:AM31"/>
+    <mergeCell ref="AN31:AS31"/>
+    <mergeCell ref="AI30:AM30"/>
+    <mergeCell ref="AN30:AS30"/>
+    <mergeCell ref="AI29:AM29"/>
+    <mergeCell ref="AN29:AS29"/>
+    <mergeCell ref="AN33:AS33"/>
+    <mergeCell ref="V33:AH33"/>
+    <mergeCell ref="AN32:AS32"/>
+    <mergeCell ref="V29:AH29"/>
+    <mergeCell ref="V30:AH30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="J32:Q32"/>
+    <mergeCell ref="J31:Q31"/>
+    <mergeCell ref="J33:Q35"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
@@ -57455,12 +57456,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="35.25" customHeight="1" thickBot="1">
-      <c r="A1" s="322" t="s">
+      <c r="A1" s="319" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="262"/>
-      <c r="C1" s="262"/>
-      <c r="D1" s="260"/>
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="266"/>
       <c r="E1" s="86"/>
       <c r="F1" s="87"/>
       <c r="G1" s="87"/>
@@ -57617,10 +57618,10 @@
       <c r="X5" s="87"/>
     </row>
     <row r="6" spans="1:24" ht="14.4">
-      <c r="A6" s="325" t="s">
+      <c r="A6" s="324" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="326"/>
+      <c r="B6" s="325"/>
       <c r="C6" s="97" t="s">
         <v>118</v>
       </c>
@@ -57649,21 +57650,21 @@
       <c r="X6" s="87"/>
     </row>
     <row r="7" spans="1:24" ht="14.4">
-      <c r="A7" s="318" t="s">
+      <c r="A7" s="322" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="319"/>
-      <c r="C7" s="329" t="s">
+      <c r="B7" s="323"/>
+      <c r="C7" s="328" t="s">
         <v>119</v>
       </c>
       <c r="D7" s="99">
         <f>CO_PO_AttainmentAnalysis!$AN$36/GradeSheet!$H$39</f>
         <v>0</v>
       </c>
-      <c r="E7" s="323"/>
-      <c r="F7" s="323"/>
-      <c r="G7" s="323"/>
-      <c r="H7" s="323"/>
+      <c r="E7" s="320"/>
+      <c r="F7" s="320"/>
+      <c r="G7" s="320"/>
+      <c r="H7" s="320"/>
       <c r="I7" s="87"/>
       <c r="J7" s="87"/>
       <c r="K7" s="87"/>
@@ -57682,19 +57683,19 @@
       <c r="X7" s="87"/>
     </row>
     <row r="8" spans="1:24" ht="14.4">
-      <c r="A8" s="325" t="s">
+      <c r="A8" s="324" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="262"/>
-      <c r="C8" s="330"/>
+      <c r="B8" s="265"/>
+      <c r="C8" s="329"/>
       <c r="D8" s="99">
         <f>CO_PO_AttainmentAnalysis!$AO$36/GradeSheet!$H$39</f>
         <v>0</v>
       </c>
-      <c r="E8" s="323"/>
-      <c r="F8" s="323"/>
-      <c r="G8" s="323"/>
-      <c r="H8" s="323"/>
+      <c r="E8" s="320"/>
+      <c r="F8" s="320"/>
+      <c r="G8" s="320"/>
+      <c r="H8" s="320"/>
       <c r="I8" s="87"/>
       <c r="J8" s="87"/>
       <c r="K8" s="87"/>
@@ -57713,19 +57714,19 @@
       <c r="X8" s="87"/>
     </row>
     <row r="9" spans="1:24" ht="14.4">
-      <c r="A9" s="318" t="s">
+      <c r="A9" s="322" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="319"/>
-      <c r="C9" s="330"/>
+      <c r="B9" s="323"/>
+      <c r="C9" s="329"/>
       <c r="D9" s="99">
         <f>CO_PO_AttainmentAnalysis!$AP$36/GradeSheet!$H$39</f>
         <v>0</v>
       </c>
-      <c r="E9" s="323"/>
-      <c r="F9" s="323"/>
-      <c r="G9" s="323"/>
-      <c r="H9" s="323"/>
+      <c r="E9" s="320"/>
+      <c r="F9" s="320"/>
+      <c r="G9" s="320"/>
+      <c r="H9" s="320"/>
       <c r="I9" s="87"/>
       <c r="J9" s="87"/>
       <c r="K9" s="87"/>
@@ -57744,19 +57745,19 @@
       <c r="X9" s="87"/>
     </row>
     <row r="10" spans="1:24" ht="14.4">
-      <c r="A10" s="318" t="s">
+      <c r="A10" s="322" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="319"/>
-      <c r="C10" s="330"/>
+      <c r="B10" s="323"/>
+      <c r="C10" s="329"/>
       <c r="D10" s="99">
         <f>CO_PO_AttainmentAnalysis!$AQ$36/GradeSheet!$H$39</f>
         <v>0</v>
       </c>
-      <c r="E10" s="323"/>
-      <c r="F10" s="323"/>
-      <c r="G10" s="323"/>
-      <c r="H10" s="323"/>
+      <c r="E10" s="320"/>
+      <c r="F10" s="320"/>
+      <c r="G10" s="320"/>
+      <c r="H10" s="320"/>
       <c r="I10" s="87"/>
       <c r="J10" s="87"/>
       <c r="K10" s="87"/>
@@ -57775,19 +57776,19 @@
       <c r="X10" s="87"/>
     </row>
     <row r="11" spans="1:24" thickBot="1">
-      <c r="A11" s="318" t="s">
+      <c r="A11" s="322" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="319"/>
-      <c r="C11" s="330"/>
+      <c r="B11" s="323"/>
+      <c r="C11" s="329"/>
       <c r="D11" s="99">
         <f>CO_PO_AttainmentAnalysis!$AR$36/GradeSheet!$H$39</f>
         <v>0</v>
       </c>
-      <c r="E11" s="323"/>
-      <c r="F11" s="323"/>
-      <c r="G11" s="323"/>
-      <c r="H11" s="323"/>
+      <c r="E11" s="320"/>
+      <c r="F11" s="320"/>
+      <c r="G11" s="320"/>
+      <c r="H11" s="320"/>
       <c r="I11" s="87"/>
       <c r="J11" s="87"/>
       <c r="K11" s="87"/>
@@ -57806,11 +57807,11 @@
       <c r="X11" s="87"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" thickBot="1">
-      <c r="A12" s="318" t="s">
+      <c r="A12" s="322" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="319"/>
-      <c r="C12" s="331"/>
+      <c r="B12" s="323"/>
+      <c r="C12" s="330"/>
       <c r="D12" s="99">
         <f>CO_PO_AttainmentAnalysis!$AS$36/GradeSheet!$H$39</f>
         <v>0</v>
@@ -57863,12 +57864,12 @@
       <c r="X13" s="87"/>
     </row>
     <row r="14" spans="1:24" ht="27" customHeight="1">
-      <c r="A14" s="332" t="s">
+      <c r="A14" s="331" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="316"/>
-      <c r="C14" s="316"/>
-      <c r="D14" s="316"/>
+      <c r="B14" s="293"/>
+      <c r="C14" s="293"/>
+      <c r="D14" s="293"/>
       <c r="E14" s="176"/>
       <c r="F14" s="176"/>
       <c r="G14" s="176"/>
@@ -57891,7 +57892,7 @@
       <c r="X14" s="87"/>
     </row>
     <row r="15" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A15" s="328"/>
+      <c r="A15" s="327"/>
       <c r="B15" s="248"/>
       <c r="C15" s="248"/>
       <c r="D15" s="249"/>
@@ -57917,7 +57918,7 @@
       <c r="X15" s="87"/>
     </row>
     <row r="16" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A16" s="327" t="s">
+      <c r="A16" s="326" t="s">
         <v>127</v>
       </c>
       <c r="B16" s="248"/>
@@ -57945,7 +57946,7 @@
       <c r="X16" s="87"/>
     </row>
     <row r="17" spans="1:24" ht="16.2">
-      <c r="A17" s="320" t="s">
+      <c r="A17" s="332" t="s">
         <v>164</v>
       </c>
       <c r="B17" s="248"/>
@@ -57973,7 +57974,7 @@
       <c r="X17" s="87"/>
     </row>
     <row r="18" spans="1:24" ht="16.2">
-      <c r="A18" s="320"/>
+      <c r="A18" s="332"/>
       <c r="B18" s="248"/>
       <c r="C18" s="248"/>
       <c r="D18" s="249"/>
@@ -58025,7 +58026,7 @@
       <c r="X19" s="87"/>
     </row>
     <row r="20" spans="1:24" ht="14.4">
-      <c r="A20" s="320"/>
+      <c r="A20" s="332"/>
       <c r="B20" s="248"/>
       <c r="C20" s="248"/>
       <c r="D20" s="249"/>
@@ -58077,7 +58078,7 @@
       <c r="X21" s="87"/>
     </row>
     <row r="22" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A22" s="320"/>
+      <c r="A22" s="332"/>
       <c r="B22" s="248"/>
       <c r="C22" s="248"/>
       <c r="D22" s="249"/>
@@ -58103,7 +58104,7 @@
       <c r="X22" s="87"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A23" s="321"/>
+      <c r="A23" s="318"/>
       <c r="B23" s="248"/>
       <c r="C23" s="248"/>
       <c r="D23" s="249"/>
@@ -58129,7 +58130,7 @@
       <c r="X23" s="87"/>
     </row>
     <row r="24" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A24" s="321"/>
+      <c r="A24" s="318"/>
       <c r="B24" s="248"/>
       <c r="C24" s="248"/>
       <c r="D24" s="249"/>
@@ -58151,7 +58152,7 @@
       <c r="X24" s="87"/>
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A25" s="321"/>
+      <c r="A25" s="318"/>
       <c r="B25" s="248"/>
       <c r="C25" s="248"/>
       <c r="D25" s="249"/>
@@ -58232,10 +58233,10 @@
       <c r="C28" s="87"/>
       <c r="D28" s="109"/>
       <c r="E28" s="166"/>
-      <c r="F28" s="324"/>
-      <c r="G28" s="323"/>
-      <c r="H28" s="323"/>
-      <c r="I28" s="323"/>
+      <c r="F28" s="321"/>
+      <c r="G28" s="320"/>
+      <c r="H28" s="320"/>
+      <c r="I28" s="320"/>
       <c r="J28" s="87"/>
       <c r="K28" s="87"/>
       <c r="L28" s="87"/>
@@ -58258,10 +58259,10 @@
       <c r="C29" s="87"/>
       <c r="D29" s="109"/>
       <c r="E29" s="166"/>
-      <c r="F29" s="323"/>
-      <c r="G29" s="323"/>
-      <c r="H29" s="323"/>
-      <c r="I29" s="323"/>
+      <c r="F29" s="320"/>
+      <c r="G29" s="320"/>
+      <c r="H29" s="320"/>
+      <c r="I29" s="320"/>
       <c r="J29" s="87"/>
       <c r="K29" s="87"/>
       <c r="L29" s="87"/>
@@ -58284,10 +58285,10 @@
       <c r="C30" s="87"/>
       <c r="D30" s="109"/>
       <c r="E30" s="166"/>
-      <c r="F30" s="323"/>
-      <c r="G30" s="323"/>
-      <c r="H30" s="323"/>
-      <c r="I30" s="323"/>
+      <c r="F30" s="320"/>
+      <c r="G30" s="320"/>
+      <c r="H30" s="320"/>
+      <c r="I30" s="320"/>
       <c r="J30" s="87"/>
       <c r="K30" s="87"/>
       <c r="L30" s="87"/>
@@ -58310,10 +58311,10 @@
       <c r="C31" s="87"/>
       <c r="D31" s="109"/>
       <c r="E31" s="166"/>
-      <c r="F31" s="323"/>
-      <c r="G31" s="323"/>
-      <c r="H31" s="323"/>
-      <c r="I31" s="323"/>
+      <c r="F31" s="320"/>
+      <c r="G31" s="320"/>
+      <c r="H31" s="320"/>
+      <c r="I31" s="320"/>
       <c r="J31" s="87"/>
       <c r="K31" s="87"/>
       <c r="L31" s="87"/>
@@ -58336,10 +58337,10 @@
       <c r="C32" s="87"/>
       <c r="D32" s="87"/>
       <c r="E32" s="166"/>
-      <c r="F32" s="323"/>
-      <c r="G32" s="323"/>
-      <c r="H32" s="323"/>
-      <c r="I32" s="323"/>
+      <c r="F32" s="320"/>
+      <c r="G32" s="320"/>
+      <c r="H32" s="320"/>
+      <c r="I32" s="320"/>
       <c r="J32" s="87"/>
       <c r="K32" s="87"/>
       <c r="L32" s="87"/>
@@ -64419,6 +64420,11 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A22:D22"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A24:D24"/>
@@ -64435,11 +64441,6 @@
     <mergeCell ref="C7:C12"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>